<commit_message>
r Please enter the commit message for your changes. Lines starting 20220520_Face_Tagger
</commit_message>
<xml_diff>
--- a/Face_Tagger/Resources/TabInfo.xlsx
+++ b/Face_Tagger/Resources/TabInfo.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahum\Documents\GitHub\Face_Tagger_Project\Face_Tagger\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE634C1-C5FA-4B54-A1B3-791383D4BF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1283" yWindow="1463" windowWidth="15390" windowHeight="9982" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24225" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Face" sheetId="1" r:id="rId1"/>
@@ -25,12 +19,12 @@
     <sheet name="Others" sheetId="10" r:id="rId10"/>
     <sheet name="Phrases" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -44,7 +38,7 @@
     <t>Shape</t>
   </si>
   <si>
-    <t>Ovalada,Redonda,Rectangular,Cuadrada,Triangular,Diamante</t>
+    <t>Ovalada,Redonda,Rectangular,Cuadrada,Triangular,Diamante, Pescado</t>
   </si>
   <si>
     <t>Combo</t>
@@ -105,13 +99,37 @@
   </si>
   <si>
     <t>{1: 'Ovalada', 2: 'Liso', 3: 'Partido a la mitad', 'Triangulo invertido': False, 'Remolino': False, 4: 'Corto', 'ovalada': False, ' redonda': True, 'exist': False, 'no exist': True, 'ovalada0': False, ' redonda1': True, 'exist2': False, 'no exist3': True, 'ovalada4': False, ' redonda5': True, 'exist6': False, 'no exist7': True, 'ovalada8': False, ' redonda9': True, 'ovalada10': False, ' redonda11': True}</t>
+  </si>
+  <si>
+    <t>00002</t>
+  </si>
+  <si>
+    <t>00024</t>
+  </si>
+  <si>
+    <t>{1: 'Cuadrada', 2: 'Liso', 3: 'Partido a la mitad', 'Triangulo invertido': False, 'Remolino': False, 4: 'Corto', 'ovalada': False, ' redonda': True, 'exist': False, 'no exist': True, 'ovalada0': False, ' redonda1': True, 'exist2': False, 'no exist3': True, 'ovalada4': False, ' redonda5': True, 'exist6': False, 'no exist7': True, 'ovalada8': False, ' redonda9': True, 'ovalada10': False, ' redonda11': True}</t>
+  </si>
+  <si>
+    <t>00003</t>
+  </si>
+  <si>
+    <t>00020</t>
+  </si>
+  <si>
+    <t>{1: 'Diamante', 2: 'Liso', 3: 'Partido a la mitad', 'Triangulo invertido': False, 'Remolino': False, 4: 'Corto', 'ovalada': False, ' redonda': True, 'exist': False, 'no exist': True, 'ovalada0': False, ' redonda1': True, 'exist2': False, 'no exist3': True, 'ovalada4': False, ' redonda5': True, 'exist6': False, 'no exist7': True, 'ovalada8': False, ' redonda9': True, 'ovalada10': False, ' redonda11': True}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,16 +137,346 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -136,24 +484,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -411,22 +1045,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="68.265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="2" max="2" width="68.2666666666667" customWidth="1"/>
+    <col min="3" max="3" width="15.1333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -453,21 +1087,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" customWidth="1"/>
-    <col min="2" max="2" width="7.19921875" customWidth="1"/>
+    <col min="1" max="1" width="7.6" customWidth="1"/>
+    <col min="2" max="2" width="7.2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -494,21 +1130,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="14.796875" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" customWidth="1"/>
+    <col min="2" max="2" width="14.8" customWidth="1"/>
+    <col min="3" max="3" width="20.2666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -525,7 +1163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -536,23 +1174,57 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.46484375" customWidth="1"/>
-    <col min="2" max="2" width="7.73046875" customWidth="1"/>
+    <col min="1" max="1" width="8.46666666666667" customWidth="1"/>
+    <col min="2" max="2" width="7.73333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -612,18 +1284,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -649,18 +1323,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -686,18 +1362,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -723,18 +1401,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -760,18 +1440,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -797,20 +1479,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="30.73046875" customWidth="1"/>
+    <col min="2" max="2" width="30.7333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -837,18 +1521,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.13333333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -874,5 +1560,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>